<commit_message>
Updated post on causal inference packages, updated teaching
</commit_message>
<xml_diff>
--- a/content/post/useful_r_packages.xlsx
+++ b/content/post/useful_r_packages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhidalgo/Dropbox (MIT)/work/website/content/post/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhidalgo/Dropbox (MIT)/website/content/post/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E93B1A-CD64-3B4E-9E1C-2C1F578C6DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0774BB63-4A52-AC4A-9B55-7EBF72493C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{CDF421F0-405A-7143-A6ED-C2528E2B33E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Package</t>
   </si>
@@ -45,19 +45,55 @@
     <t>lfe</t>
   </si>
   <si>
-    <t>https://github.com/sgaure/lfe</t>
-  </si>
-  <si>
     <t xml:space="preserve">This package is a workhorse package for regression modeling. One of its chief strengths is that it allows for the  fast estimation of models with high dimensional fixed effects. It also has functionality for instrumental variables regression and allows for heteroskedastic/cluster robust standard errors.  </t>
   </si>
   <si>
-    <t>eventStudy</t>
-  </si>
-  <si>
-    <t>https://github.com/setzler/eventStudy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This package implements panel event studies. </t>
+    <t>estimatr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This package has my goto drop-in replacement for `lm`: `robust_lm` which conveniently allows for robust and clustered standard errors. Also includes other estimators commonly used in designed-based inference. </t>
+  </si>
+  <si>
+    <t>sensemakr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R package implementing the sensitivity analysis methods for unmeasured confounding proposed in [Cinelli and Hazlett](https://doi.org/10.1111/rssb.12348). This is the first approach I suggest to students interested in implementing a sensitivity analysis. </t>
+  </si>
+  <si>
+    <t>rdrobust</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=sensemakr</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=estimatr</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=lfe</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=rdrobust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implements a suite of estimation methods, bandwidth selection algorthims, and graphical tools for regression discontinuity designs. </t>
+  </si>
+  <si>
+    <t>gsynth</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=gsynth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides recent panel-data estimators that go beyond standard fixed effects models, including interactive fixed effects models and matrix completion methods. </t>
+  </si>
+  <si>
+    <t>PanelMatch</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=PanelMatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implements generalized diffence-in-differences  estimators that avoid some of the recently identified [problems](https://www.nber.org/papers/w25018) with two-way fixed effect models. </t>
   </si>
 </sst>
 </file>
@@ -115,11 +151,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,23 +474,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73D779D-C656-564C-8340-2D00DCA9F4F3}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="85.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -462,28 +503,77 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{DC58D8AA-B372-5241-AE6D-FAA7741E310D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FA11B4B0-C673-0F43-B0B7-DF0653C3577E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6B9464EE-6366-A146-965C-9A9B0226BF3D}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{1B1DB204-7921-7E40-B3E2-3602129F5D39}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{61DA97F5-2048-4548-81A6-756F592C26DC}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{D90B2BED-A467-374B-AD9F-FE0916533A30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>